<commit_message>
EDM-4: improved function for updating and reading data from Excel
</commit_message>
<xml_diff>
--- a/ExampleList.xlsx
+++ b/ExampleList.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Всякая всячина\Java\EDM-Excel-Document-Manager-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6C358-192F-4358-9CFA-86EE721FA690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1300CFD0-17ED-4F84-BE97-354D10BDA53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2484" yWindow="3612" windowWidth="17100" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3132" yWindow="3672" windowWidth="17100" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Документы" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,15 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
-    <t>папапа</t>
+    <t>Доверенность</t>
+  </si>
+  <si>
+    <t>17.01.2024</t>
+  </si>
+  <si>
+    <t>26.01.2024</t>
+  </si>
+  <si>
+    <t>fdfd</t>
+  </si>
+  <si>
+    <t>03.01.2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd.mm.yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,9 +79,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -346,37 +371,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>23131</v>
+      <c r="A1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>312321.0</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1">
-        <v>45323</v>
-      </c>
-      <c r="E1" s="1">
-        <v>45324</v>
-      </c>
-      <c r="F1">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>12312.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* EDM-5: crud functionality implemented, patch added * EDM-5: UI is divided into components, improving business logic
</commit_message>
<xml_diff>
--- a/ExampleList.xlsx
+++ b/ExampleList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Всякая всячина\Java\EDM-Excel-Document-Manager-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1300CFD0-17ED-4F84-BE97-354D10BDA53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350CFD5-F970-441F-9A32-03F33B136450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3132" yWindow="3672" windowWidth="17100" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,21 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
-  <si>
-    <t>Доверенность</t>
-  </si>
-  <si>
-    <t>17.01.2024</t>
-  </si>
-  <si>
-    <t>26.01.2024</t>
-  </si>
-  <si>
-    <t>fdfd</t>
-  </si>
-  <si>
-    <t>03.01.2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+  <si>
+    <t>gfgfg</t>
+  </si>
+  <si>
+    <t>05.01.2024</t>
+  </si>
+  <si>
+    <t>21.01.2024</t>
+  </si>
+  <si>
+    <t>gfgfgf</t>
+  </si>
+  <si>
+    <t>13.01.2024</t>
+  </si>
+  <si>
+    <t>20.01.2024</t>
+  </si>
+  <si>
+    <t>hjhhk</t>
+  </si>
+  <si>
+    <t>12.01.2024</t>
+  </si>
+  <si>
+    <t>04.02.2024</t>
+  </si>
+  <si>
+    <t>Абоба</t>
+  </si>
+  <si>
+    <t>Еще одна абоба</t>
+  </si>
+  <si>
+    <t>fgfgfgfgg</t>
+  </si>
+  <si>
+    <t>14.01.2021</t>
+  </si>
+  <si>
+    <t>28.01.2024</t>
   </si>
 </sst>
 </file>
@@ -79,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -89,6 +116,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -371,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,69 +415,81 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>312321.0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>12312.0</v>
+        <v>1232.0</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>2</v>
+      <c r="E2" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="F2" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>13123.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="n">
         <v>1.0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* EDM-6: added dynamic change of days until a document is overdue * EDM-6: Improved overall program performance
</commit_message>
<xml_diff>
--- a/ExampleList.xlsx
+++ b/ExampleList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Всякая всячина\Java\EDM-Excel-Document-Manager-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350CFD5-F970-441F-9A32-03F33B136450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C302AE-5F31-4617-B888-606698B1DE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3132" yWindow="3672" windowWidth="17100" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,48 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
-  <si>
-    <t>gfgfg</t>
-  </si>
-  <si>
-    <t>05.01.2024</t>
-  </si>
-  <si>
-    <t>21.01.2024</t>
-  </si>
-  <si>
-    <t>gfgfgf</t>
-  </si>
-  <si>
-    <t>13.01.2024</t>
-  </si>
-  <si>
-    <t>20.01.2024</t>
-  </si>
-  <si>
-    <t>hjhhk</t>
-  </si>
-  <si>
-    <t>12.01.2024</t>
-  </si>
-  <si>
-    <t>04.02.2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+  <si>
+    <t>ававааввпв</t>
+  </si>
+  <si>
+    <t>25.01.2024</t>
+  </si>
+  <si>
+    <t>26.01.2024</t>
   </si>
   <si>
     <t>Абоба</t>
   </si>
   <si>
-    <t>Еще одна абоба</t>
-  </si>
-  <si>
-    <t>fgfgfgfgg</t>
-  </si>
-  <si>
-    <t>14.01.2021</t>
-  </si>
-  <si>
-    <t>28.01.2024</t>
+    <t>ававпвпв</t>
+  </si>
+  <si>
+    <t>31.01.2024</t>
+  </si>
+  <si>
+    <t>29.01.2024</t>
   </si>
 </sst>
 </file>
@@ -106,18 +85,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -403,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,39 +394,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>1232.0</v>
+        <v>312312.0</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>13123.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -460,28 +411,21 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>1.23123123E8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>

</xml_diff>

<commit_message>
EDM-7: added warnings about document overdue and updated README.md
</commit_message>
<xml_diff>
--- a/ExampleList.xlsx
+++ b/ExampleList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Всякая всячина\Java\EDM-Excel-Document-Manager-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C302AE-5F31-4617-B888-606698B1DE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C19ED6A-57A1-49E5-803D-9409F61C2759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3132" yWindow="3672" windowWidth="17100" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,36 +25,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
-  <si>
-    <t>ававааввпв</t>
-  </si>
-  <si>
-    <t>25.01.2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+  <si>
+    <t>выавыавыава</t>
   </si>
   <si>
     <t>26.01.2024</t>
   </si>
   <si>
-    <t>Абоба</t>
-  </si>
-  <si>
-    <t>ававпвпв</t>
-  </si>
-  <si>
     <t>31.01.2024</t>
   </si>
   <si>
+    <t>аваыаы</t>
+  </si>
+  <si>
     <t>29.01.2024</t>
+  </si>
+  <si>
+    <t>вавыаывыва</t>
+  </si>
+  <si>
+    <t>30.01.2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd.mm.yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -85,18 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -377,63 +369,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-  </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>2.1312312E7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>312312.0</v>
+        <v>1.3213213E7</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1.23123123E8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>